<commit_message>
11 parameters. Sensitivity analysis was done based on rest data. Parameters in all layers of the myocardium are chosen for parameter estimation.
</commit_message>
<xml_diff>
--- a/Sensitivity.xlsx
+++ b/Sensitivity.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Params" sheetId="4" r:id="rId1"/>
     <sheet name="CoV" sheetId="1" r:id="rId2"/>
     <sheet name="Sensitivity1" sheetId="2" r:id="rId3"/>
     <sheet name="Sensitivity2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sensitivity8" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
   <si>
     <t>endo</t>
   </si>
@@ -129,11 +130,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -149,12 +147,149 @@
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -442,201 +577,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>11.87184929</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>1.5582333500000001</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>1.05098446</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>81.118940370000004</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>82.353021659999996</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>120.38092107999999</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1.89700187</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>11.682823190000001</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1.90550636</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>-8.5750769600000005</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>1.20888157</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>20.736283159999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>50.862582660000001</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>133.57678379999999</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>175.43903226</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>199.55879150999999</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>68.60612021</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>107.65169582999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>190.07671963999999</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>318.08196193999999</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>272.89492166999997</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>10.64161129</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>13.923384670000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>27.482876059999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>0.14024027</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>8.5278740000000006E-2</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.21975875</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>0.1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>1.5608189999999999E-2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>2.8897800000000002E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>-2.6895914900000002</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>-3.2958286800000001</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>-9.7351343099999994</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>84.202084990000003</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>99.999999990000006</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>99.999999990000006</v>
       </c>
     </row>
@@ -665,85 +800,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3">
         <v>0.43058739438984001</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>0.93246815522773996</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>1.0974922071988999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>8.0023737394409503E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.126599183618233</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.23185981155542201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.66895868160233496</v>
       </c>
       <c r="D4" s="3">
         <v>0.30851503187395002</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.87316240343186802</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3">
         <v>0.434129781699721</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>1.4255969468232901</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>7.6884767100044096</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3">
@@ -757,40 +892,40 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.57407579011965704</v>
       </c>
       <c r="D7" s="3">
         <v>0.346574132303828</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.52462984346833896</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.270737929654291</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.246478126715762</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>0.20079746937718401</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3">
@@ -804,62 +939,62 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.54324851669711605</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>1.060479098354</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.81377785048887696</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="3">
         <v>0.46225807872713698</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>1.2900929756038699</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>1.8751531661817</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>1.87752505784941</v>
       </c>
       <c r="D12" s="3">
         <v>0.34051874236125201</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.52637612440948101</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>0.14334497741688099</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0.19935737512785801</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>0.16645139061696901</v>
       </c>
     </row>
@@ -888,206 +1023,206 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0.37144339328263998</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>9.0875192195452897E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>5.87191818273015E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>2.5919435839191598</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>7.3219489624443607E-2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.120440239736626</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0.11514922318646199</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.112665035208974</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.19978947066625699</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>8.73555989419285E-2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>7.63251665113511E-2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.32454623238151498</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>6.7320581274987301E-2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1.62645564725087</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>5.8222243161316101</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>0.137414219566033</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.68278583945092097</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>2.9126059303077398</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>0.223390875533649</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>0.26597631388364601</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>1.15698159092091</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>9.0825601332383002E-2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.54145310589610696</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>3.5904113130731701</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>3.2492655471896302E-2</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>0.13373405413797099</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>0.47539350992912599</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>3.3682132447728899E-2</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>4.5363121588720801E-2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>0.103948124133663</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>7.7525139292257406E-2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>0.51490381493678705</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>2.5828055044212999</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>0.382191272417163</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>0.202728069159749</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>8.2845264848049299E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
+      <c r="C14" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1103,8 +1238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,201 +1249,201 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>6.4571721080314198E-2</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2.42237728791267E-2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1.6829801842614001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.34141291921181199</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3.6354822210695699E-2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>2.4540468922633601E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>5.7202072151149801E-2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1.85598681696971E-2</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>3.68211655799053E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>3.8431969811627997E-2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>2.1644130037777699E-2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>4.8126441759213302E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>2.2135948787553299E-2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.48602265290095897</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>3.8335088670566002E-2</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.21601830452214801</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>0.26152973694059001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>3.3652704742304203E-2</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.104438760691126</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.11081022371473399</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>3.2371272899174602E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.15404929380674501</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>0.28548695939138902</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1.03532437268081E-2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>3.4709414110003903E-2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>5.1335614485625299E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>3.6705308391566799E-2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>2.8815822159745701E-2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>4.2611161729549402E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>1.52945973060376E-2</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>0.158134818451026</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.30893582423926103</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>4.1937168335872702E-2</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>6.3396219484393598E-2</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>1.8263989081551201E-2</v>
       </c>
     </row>
@@ -1320,4 +1455,237 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4.7486971020258797E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2.0062406413766599E-2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5.9711471765740301E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4.9547239946083899E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3.3120399505278203E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.2532744234877999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.163469890639E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.10741016174375E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.157561124314096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3.1294330699889503E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.43475631308516299</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.82826145756501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3.2542005912193403E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.17430571074474799</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.2537295020244901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9.1932013551008301E-2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.21499696699075699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2.9644459518474001E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>3.5122073235181898E-2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5.05566478381465E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1.45197804450901E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2.02918340172847E-2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>2.29459828556592E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7">
+        <v>3.1284771505818001E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>9.0145546912524993E-2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.26209999127837702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:E13">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Variable Sv case set up and ready for parameter estimation. The nominal parameters are taken to be those of Pig #3
</commit_message>
<xml_diff>
--- a/Sensitivity.xlsx
+++ b/Sensitivity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="4"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Params" sheetId="4" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="Sensitivity1" sheetId="2" r:id="rId3"/>
     <sheet name="Sensitivity2" sheetId="3" r:id="rId4"/>
     <sheet name="Sensitivity8" sheetId="5" r:id="rId5"/>
+    <sheet name="Sensitivity10" sheetId="7" r:id="rId6"/>
+    <sheet name="Sensitivity11" sheetId="6" r:id="rId7"/>
+    <sheet name="Sensitivity10+11" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="18">
   <si>
     <t>endo</t>
   </si>
@@ -130,7 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -153,12 +156,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -171,11 +177,31 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C6500"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -241,41 +267,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -590,7 +586,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -607,7 +603,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -622,7 +618,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -637,7 +633,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -652,7 +648,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -669,7 +665,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -684,7 +680,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -699,7 +695,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -716,7 +712,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -731,7 +727,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -746,7 +742,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -761,7 +757,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -813,7 +809,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -830,7 +826,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -845,7 +841,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -860,7 +856,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -875,7 +871,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -892,7 +888,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -907,7 +903,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -922,7 +918,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -939,7 +935,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -954,7 +950,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -969,7 +965,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -984,7 +980,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1036,7 +1032,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1053,7 +1049,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1068,7 +1064,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1083,7 +1079,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1098,7 +1094,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1115,7 +1111,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1126,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1145,7 +1141,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1162,7 +1158,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1177,7 +1173,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1188,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1207,7 +1203,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1262,7 +1258,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1279,7 +1275,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1294,7 +1290,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1309,7 +1305,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1324,7 +1320,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1341,7 +1337,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1352,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1371,7 +1367,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1388,7 +1384,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1403,7 +1399,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1414,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1433,7 +1429,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1461,7 +1457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
@@ -1484,7 +1480,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1501,7 +1497,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1512,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1531,7 +1527,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1546,7 +1542,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1563,7 +1559,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1578,7 +1574,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1593,7 +1589,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1610,7 +1606,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1625,7 +1621,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1640,7 +1636,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1655,7 +1651,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1676,13 +1672,733 @@
     <mergeCell ref="A9:A13"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:E13">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1.3464159011691901E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.9633124542735199E-2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>2.8758027097512399E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2.7637682573484399E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3.9975290439744397E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>5.4075775648697297E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3.9418750830657601E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.32143903029548E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3.7727820953092503E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>2.5716330770578E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.94307060995286895</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.67375641739067604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7.5771111133918403E-3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9.2772737399238903E-3</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.17756217213018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3.4771723043826398E-2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>8.3890222561279801E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7">
+        <v>3.6900373638763397E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>6.7582294950693901E-3</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1.7150628671723699E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1.37298083254783E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4.0118760461468603E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.14495523399605501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:E13">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7">
+        <v>8.1072153066678296E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>3.0823852432039101E-2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>9.2200554972645798E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2.2027645051356001E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1.22635685080807E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>7.6555466679572104E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.4641574979928899E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.0987489256530701E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.25392441359558798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <v>8.0647409242546805E-3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.441363492808939</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.8547127603168601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7.9575154261208193E-3</v>
+      </c>
+      <c r="D7" s="7">
+        <v>8.2181506411947297E-2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.14193335754273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9.9714430679687494E-2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.191769312046733</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7">
+        <v>9.8464964016667603E-3</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2.39842311838224E-2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4.7444703336942798E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2.02882150737464E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1.6764476143105E-2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>9.3383642660929793E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1.5875293793364002E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>7.2884047150292605E-2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.31703372810279301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:E13">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7">
+        <f>Sensitivity10!C2+Sensitivity11!C2</f>
+        <v>9.4536312078370197E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <f>Sensitivity10!D2+Sensitivity11!D2</f>
+        <v>5.0456976974774304E-2</v>
+      </c>
+      <c r="E2" s="7">
+        <f>Sensitivity10!E2+Sensitivity11!E2</f>
+        <v>3.7978082594776981E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <f>Sensitivity10!C3+Sensitivity11!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <f>Sensitivity10!D3+Sensitivity11!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <f>Sensitivity10!E3+Sensitivity11!E3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7">
+        <f>Sensitivity10!C4+Sensitivity11!C4</f>
+        <v>4.9665327624840397E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <f>Sensitivity10!D4+Sensitivity11!D4</f>
+        <v>5.2238858947825095E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <f>Sensitivity10!E4+Sensitivity11!E4</f>
+        <v>6.1731322316654506E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7">
+        <f>Sensitivity10!C5+Sensitivity11!C5</f>
+        <v>5.40603258105865E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <f>Sensitivity10!D5+Sensitivity11!D5</f>
+        <v>2.4201879559485502E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <f>Sensitivity10!E5+Sensitivity11!E5</f>
+        <v>0.2916522345486805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7">
+        <f>Sensitivity10!C6+Sensitivity11!C6</f>
+        <v>3.378107169483268E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <f>Sensitivity10!D6+Sensitivity11!D6</f>
+        <v>1.3844341027618079</v>
+      </c>
+      <c r="E6" s="7">
+        <f>Sensitivity10!E6+Sensitivity11!E6</f>
+        <v>2.5284691777075361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <f>Sensitivity10!C7+Sensitivity11!C7</f>
+        <v>1.553462653951266E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <f>Sensitivity10!D7+Sensitivity11!D7</f>
+        <v>9.1458780151871186E-2</v>
+      </c>
+      <c r="E7" s="7">
+        <f>Sensitivity10!E7+Sensitivity11!E7</f>
+        <v>1.3194955296729098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <f>Sensitivity10!C8+Sensitivity11!C8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <f>Sensitivity10!D8+Sensitivity11!D8</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <f>Sensitivity10!E8+Sensitivity11!E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="7">
+        <f>Sensitivity10!C9+Sensitivity11!C9</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <f>Sensitivity10!D9+Sensitivity11!D9</f>
+        <v>0.13448615372351388</v>
+      </c>
+      <c r="E9" s="7">
+        <f>Sensitivity10!E9+Sensitivity11!E9</f>
+        <v>0.27565953460801279</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7">
+        <f>Sensitivity10!C10+Sensitivity11!C10</f>
+        <v>4.6746870040430155E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <f>Sensitivity10!D10+Sensitivity11!D10</f>
+        <v>3.0742460678891789E-2</v>
+      </c>
+      <c r="E10" s="7">
+        <f>Sensitivity10!E10+Sensitivity11!E10</f>
+        <v>6.4595332008666489E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <f>Sensitivity10!C11+Sensitivity11!C11</f>
+        <v>3.4018023399224703E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <f>Sensitivity10!D11+Sensitivity11!D11</f>
+        <v>1.6764476143105E-2</v>
+      </c>
+      <c r="E11" s="7">
+        <f>Sensitivity10!E11+Sensitivity11!E11</f>
+        <v>9.3383642660929793E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="7">
+        <f>Sensitivity10!C12+Sensitivity11!C12</f>
+        <v>5.5994054254832601E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <f>Sensitivity10!D12+Sensitivity11!D12</f>
+        <v>2.0728840471502927</v>
+      </c>
+      <c r="E12" s="7">
+        <f>Sensitivity10!E12+Sensitivity11!E12</f>
+        <v>0.46198896209884799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7">
+        <f>Sensitivity10!C13+Sensitivity11!C13</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <f>Sensitivity10!D13+Sensitivity11!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <f>Sensitivity10!E13+Sensitivity11!E13</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A13"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2:E13">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>